<commit_message>
fix : 아이템data /slot ui
</commit_message>
<xml_diff>
--- a/program/1S3B/RawData/Item_Data.xlsx
+++ b/program/1S3B/RawData/Item_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\STIKA\Unity\1S3B\program\1S3B\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83FCC6B-56AB-4DE5-A82B-8E5DE2E0674B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1857E7C6-04EF-495D-B1B7-F4FBD2C135A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29820" yWindow="555" windowWidth="23460" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,50 +82,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>당근</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>토마토</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>딸기</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>호박</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>옥수수</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>감자</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>수박</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>무</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>양배추</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>밀</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>가지</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Path</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -183,6 +139,50 @@
   </si>
   <si>
     <t>Crops/Seeds/StrawberrySeed</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>당근씨앗</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>호박씨앗</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>감자씨앗</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>수박씨앗</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>무씨앗</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>양배추씨앗</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>밀씨앗</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>가지씨앗</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>옥수수씨앗</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>토마토씨앗</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>딸기씨앗</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -840,7 +840,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -866,13 +866,13 @@
         <v>6</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -884,7 +884,7 @@
         <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
@@ -995,11 +995,11 @@
       <c r="B6" s="1">
         <v>10002001</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
+      <c r="C6" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>16</v>
@@ -1017,18 +1017,18 @@
         <v>100</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>10002002</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>16</v>
@@ -1046,18 +1046,18 @@
         <v>100</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>10002003</v>
       </c>
-      <c r="C8" t="s">
-        <v>22</v>
+      <c r="C8" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>16</v>
@@ -1075,18 +1075,18 @@
         <v>100</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>10002004</v>
       </c>
-      <c r="C9" t="s">
-        <v>23</v>
+      <c r="C9" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>16</v>
@@ -1104,18 +1104,18 @@
         <v>100</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>10002005</v>
       </c>
-      <c r="C10" t="s">
-        <v>24</v>
+      <c r="C10" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>16</v>
@@ -1133,18 +1133,18 @@
         <v>100</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>10002006</v>
       </c>
-      <c r="C11" t="s">
-        <v>25</v>
+      <c r="C11" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>16</v>
@@ -1162,18 +1162,18 @@
         <v>100</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>10002007</v>
       </c>
-      <c r="C12" t="s">
-        <v>26</v>
+      <c r="C12" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>16</v>
@@ -1191,7 +1191,7 @@
         <v>100</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
@@ -1199,10 +1199,10 @@
         <v>10003001</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>16</v>
@@ -1220,18 +1220,18 @@
         <v>100</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>10003002</v>
       </c>
-      <c r="C14" t="s">
-        <v>21</v>
+      <c r="C14" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>16</v>
@@ -1249,18 +1249,18 @@
         <v>100</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>10003003</v>
       </c>
-      <c r="C15" t="s">
-        <v>18</v>
+      <c r="C15" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>16</v>
@@ -1278,18 +1278,18 @@
         <v>100</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>10003004</v>
       </c>
-      <c r="C16" t="s">
-        <v>19</v>
+      <c r="C16" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>16</v>
@@ -1307,7 +1307,7 @@
         <v>100</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat : 물줄때 흔들리게 dropItemSprite
</commit_message>
<xml_diff>
--- a/program/1S3B/RawData/Item_Data.xlsx
+++ b/program/1S3B/RawData/Item_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\STIKA\Unity\1S3B\program\1S3B\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4B92FD-C4BE-4E1B-A293-4B39EE115ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10BB313-C218-4464-8290-12538F91F503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
   <si>
     <t>SellGold</t>
   </si>
@@ -219,6 +219,38 @@
   </si>
   <si>
     <t>Equip/Sword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나무</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나무를 베서 나온 나무조각. 건물을 짓거나 제작할 때 사용된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돌을 캐서 나온 돌조각. 건물을 짓거나 제작할 때 사용된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wood</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stone</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -873,10 +905,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1439,6 +1471,70 @@
         <v>44</v>
       </c>
     </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>20001001</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18">
+        <v>-1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>1000</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <v>20001002</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19">
+        <v>-1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>1000</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>

<commit_message>
feat : EquipType, Equip별 테스트데이터
UI에서 아이콘만들기 전까지
</commit_message>
<xml_diff>
--- a/program/1S3B/RawData/Item_Data.xlsx
+++ b/program/1S3B/RawData/Item_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\STIKA\Unity\1S3B\program\1S3B\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A13E90F-E1CA-4365-9131-31C413CE1297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCF8612-28B3-4B0F-9944-4F1EE0A68933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28965" yWindow="990" windowWidth="23460" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="88">
   <si>
     <t>SellGold</t>
   </si>
@@ -340,6 +340,26 @@
   <si>
     <t>독 버섯</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EquipType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hoe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>PickAxe</t>
+  </si>
+  <si>
+    <t>Axe</t>
+  </si>
+  <si>
+    <t>Sword</t>
   </si>
 </sst>
 </file>
@@ -993,10 +1013,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1005,14 +1025,15 @@
     <col min="2" max="2" width="10.125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="74.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1029,25 +1050,28 @@
         <v>5</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
       <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" s="4">
         <v>1001</v>
       </c>
@@ -1060,26 +1084,29 @@
       <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2">
-        <v>-1</v>
+      <c r="F2" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="5">
+      <c r="L2" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B3" s="4">
         <v>1002</v>
       </c>
@@ -1092,26 +1119,29 @@
       <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="F3">
-        <v>-1</v>
+      <c r="F3" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>1</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="5">
+      <c r="L3" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <v>1003</v>
       </c>
@@ -1124,26 +1154,29 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="F4">
-        <v>-1</v>
+      <c r="F4" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>1</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K4" s="5">
+      <c r="L4" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <v>1004</v>
       </c>
@@ -1156,26 +1189,29 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F5">
-        <v>-1</v>
+      <c r="F5" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <v>1</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <v>1005</v>
       </c>
@@ -1188,26 +1224,29 @@
       <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="F6">
-        <v>-1</v>
+      <c r="F6" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
         <v>1</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="K6" s="5">
+      <c r="L6" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>2001</v>
       </c>
@@ -1220,26 +1259,29 @@
       <c r="E7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
+        <v>-1</v>
+      </c>
+      <c r="G7" s="1">
         <v>1</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>100</v>
-      </c>
-      <c r="J7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>100</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>2002</v>
       </c>
@@ -1252,26 +1294,29 @@
       <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
+        <v>-1</v>
+      </c>
+      <c r="G8" s="1">
         <v>2</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>100</v>
-      </c>
-      <c r="J8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>100</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="L8" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>2003</v>
       </c>
@@ -1284,26 +1329,29 @@
       <c r="E9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
+        <v>-1</v>
+      </c>
+      <c r="G9" s="1">
         <v>3</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>100</v>
-      </c>
-      <c r="J9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>100</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>2004</v>
       </c>
@@ -1316,26 +1364,29 @@
       <c r="E10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
+        <v>-1</v>
+      </c>
+      <c r="G10" s="1">
         <v>4</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>100</v>
-      </c>
-      <c r="J10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>100</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>2005</v>
       </c>
@@ -1348,26 +1399,29 @@
       <c r="E11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11">
+        <v>-1</v>
+      </c>
+      <c r="G11" s="1">
         <v>5</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>100</v>
-      </c>
-      <c r="J11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>100</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>2006</v>
       </c>
@@ -1380,26 +1434,29 @@
       <c r="E12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12">
+        <v>-1</v>
+      </c>
+      <c r="G12" s="1">
         <v>6</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>100</v>
-      </c>
-      <c r="J12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>100</v>
+      </c>
+      <c r="K12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>2007</v>
       </c>
@@ -1412,26 +1469,29 @@
       <c r="E13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
+        <v>-1</v>
+      </c>
+      <c r="G13" s="1">
         <v>7</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>100</v>
-      </c>
-      <c r="J13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>100</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>3001</v>
       </c>
@@ -1444,26 +1504,29 @@
       <c r="E14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
+        <v>-1</v>
+      </c>
+      <c r="G14" s="1">
         <v>101</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>100</v>
-      </c>
-      <c r="J14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>100</v>
+      </c>
+      <c r="K14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="L14" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>3002</v>
       </c>
@@ -1476,26 +1539,29 @@
       <c r="E15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15">
+        <v>-1</v>
+      </c>
+      <c r="G15" s="1">
         <v>102</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>100</v>
-      </c>
-      <c r="J15" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>100</v>
+      </c>
+      <c r="K15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="L15" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>3003</v>
       </c>
@@ -1508,26 +1574,29 @@
       <c r="E16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16">
+        <v>-1</v>
+      </c>
+      <c r="G16" s="1">
         <v>103</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>100</v>
-      </c>
-      <c r="J16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>100</v>
+      </c>
+      <c r="K16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="L16" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>3004</v>
       </c>
@@ -1540,26 +1609,29 @@
       <c r="E17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17">
+        <v>-1</v>
+      </c>
+      <c r="G17" s="1">
         <v>104</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>100</v>
-      </c>
-      <c r="J17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>100</v>
+      </c>
+      <c r="K17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>4001</v>
       </c>
@@ -1576,22 +1648,25 @@
         <v>-1</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>100</v>
-      </c>
-      <c r="J18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>100</v>
+      </c>
+      <c r="K18" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>4002</v>
       </c>
@@ -1608,22 +1683,25 @@
         <v>-1</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>100</v>
-      </c>
-      <c r="J19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>100</v>
+      </c>
+      <c r="K19" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>5001</v>
       </c>
@@ -1640,22 +1718,25 @@
         <v>-1</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>100</v>
-      </c>
-      <c r="J20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>100</v>
+      </c>
+      <c r="K20" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="K20" s="5">
+      <c r="L20" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
         <v>5002</v>
       </c>
@@ -1672,22 +1753,25 @@
         <v>-1</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>100</v>
-      </c>
-      <c r="J21" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>100</v>
+      </c>
+      <c r="K21" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="K21" s="5">
+      <c r="L21" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
         <v>5003</v>
       </c>
@@ -1704,22 +1788,25 @@
         <v>-1</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22">
-        <v>100</v>
-      </c>
-      <c r="J22" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>100</v>
+      </c>
+      <c r="K22" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="K22" s="5">
+      <c r="L22" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>5004</v>
       </c>
@@ -1736,22 +1823,25 @@
         <v>-1</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>100</v>
-      </c>
-      <c r="J23" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>100</v>
+      </c>
+      <c r="K23" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="K23" s="5">
+      <c r="L23" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
         <v>5005</v>
       </c>
@@ -1768,22 +1858,25 @@
         <v>-1</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
-        <v>100</v>
-      </c>
-      <c r="J24" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>100</v>
+      </c>
+      <c r="K24" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="K24" s="5">
+      <c r="L24" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
         <v>5006</v>
       </c>
@@ -1800,22 +1893,25 @@
         <v>-1</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25">
-        <v>100</v>
-      </c>
-      <c r="J25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>100</v>
+      </c>
+      <c r="K25" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="K25" s="5">
+      <c r="L25" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>5007</v>
       </c>
@@ -1832,22 +1928,25 @@
         <v>-1</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26">
-        <v>100</v>
-      </c>
-      <c r="J26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>100</v>
+      </c>
+      <c r="K26" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="K26" s="5">
+      <c r="L26" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
         <v>5101</v>
       </c>
@@ -1864,22 +1963,25 @@
         <v>-1</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27">
-        <v>100</v>
-      </c>
-      <c r="J27" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>100</v>
+      </c>
+      <c r="K27" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="K27" s="5">
+      <c r="L27" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
         <v>5102</v>
       </c>
@@ -1896,22 +1998,25 @@
         <v>-1</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28">
-        <v>100</v>
-      </c>
-      <c r="J28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>100</v>
+      </c>
+      <c r="K28" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="K28" s="5">
+      <c r="L28" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" s="1">
         <v>5103</v>
       </c>
@@ -1928,22 +2033,25 @@
         <v>-1</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H29">
         <v>0</v>
       </c>
       <c r="I29">
-        <v>100</v>
-      </c>
-      <c r="J29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>100</v>
+      </c>
+      <c r="K29" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="K29" s="5">
+      <c r="L29" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" s="1">
         <v>5104</v>
       </c>
@@ -1960,22 +2068,25 @@
         <v>-1</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30">
-        <v>100</v>
-      </c>
-      <c r="J30" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>100</v>
+      </c>
+      <c r="K30" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="K30" s="5">
+      <c r="L30" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="1">
         <v>5105</v>
       </c>
@@ -1992,22 +2103,25 @@
         <v>-1</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H31">
         <v>0</v>
       </c>
       <c r="I31">
-        <v>100</v>
-      </c>
-      <c r="J31" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>100</v>
+      </c>
+      <c r="K31" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="K31" s="5">
+      <c r="L31" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" s="1">
         <v>5106</v>
       </c>
@@ -2024,22 +2138,25 @@
         <v>-1</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H32">
         <v>0</v>
       </c>
       <c r="I32">
-        <v>100</v>
-      </c>
-      <c r="J32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>100</v>
+      </c>
+      <c r="K32" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="K32" s="5">
+      <c r="L32" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" s="1">
         <v>5201</v>
       </c>
@@ -2056,22 +2173,25 @@
         <v>-1</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
       <c r="I33">
-        <v>100</v>
-      </c>
-      <c r="J33" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>100</v>
+      </c>
+      <c r="K33" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="K33" s="5">
+      <c r="L33" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="1">
         <v>5202</v>
       </c>
@@ -2088,22 +2208,25 @@
         <v>-1</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H34">
         <v>0</v>
       </c>
       <c r="I34">
-        <v>100</v>
-      </c>
-      <c r="J34" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>100</v>
+      </c>
+      <c r="K34" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="K34" s="5">
+      <c r="L34" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" s="1">
         <v>5203</v>
       </c>
@@ -2120,22 +2243,25 @@
         <v>-1</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H35">
         <v>0</v>
       </c>
       <c r="I35">
-        <v>100</v>
-      </c>
-      <c r="J35" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>100</v>
+      </c>
+      <c r="K35" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="K35" s="5">
+      <c r="L35" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" s="1">
         <v>5204</v>
       </c>
@@ -2152,22 +2278,25 @@
         <v>-1</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H36">
         <v>0</v>
       </c>
       <c r="I36">
-        <v>100</v>
-      </c>
-      <c r="J36" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>100</v>
+      </c>
+      <c r="K36" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="K36" s="5">
+      <c r="L36" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" s="1">
         <v>5205</v>
       </c>
@@ -2184,22 +2313,25 @@
         <v>-1</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H37">
         <v>0</v>
       </c>
       <c r="I37">
-        <v>100</v>
-      </c>
-      <c r="J37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>100</v>
+      </c>
+      <c r="K37" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="K37" s="5">
+      <c r="L37" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38" s="1">
         <v>5206</v>
       </c>
@@ -2216,22 +2348,25 @@
         <v>-1</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="I38">
-        <v>100</v>
-      </c>
-      <c r="J38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>100</v>
+      </c>
+      <c r="K38" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="K38" s="5">
+      <c r="L38" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" s="1">
         <v>5301</v>
       </c>
@@ -2248,22 +2383,25 @@
         <v>-1</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H39">
         <v>0</v>
       </c>
       <c r="I39">
-        <v>100</v>
-      </c>
-      <c r="J39" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>100</v>
+      </c>
+      <c r="K39" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="K39" s="5">
+      <c r="L39" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" s="1">
         <v>5302</v>
       </c>
@@ -2280,22 +2418,25 @@
         <v>-1</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H40">
         <v>0</v>
       </c>
       <c r="I40">
-        <v>100</v>
-      </c>
-      <c r="J40" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>100</v>
+      </c>
+      <c r="K40" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="K40" s="5">
+      <c r="L40" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B41" s="1">
         <v>5303</v>
       </c>
@@ -2312,22 +2453,25 @@
         <v>-1</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H41">
         <v>0</v>
       </c>
       <c r="I41">
-        <v>100</v>
-      </c>
-      <c r="J41" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>100</v>
+      </c>
+      <c r="K41" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="K41" s="5">
+      <c r="L41" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B42" s="1">
         <v>5304</v>
       </c>
@@ -2344,18 +2488,21 @@
         <v>-1</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H42">
         <v>0</v>
       </c>
       <c r="I42">
-        <v>100</v>
-      </c>
-      <c r="J42" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>100</v>
+      </c>
+      <c r="K42" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="K42" s="5">
+      <c r="L42" s="5">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat : playerInput, NaturePoint
</commit_message>
<xml_diff>
--- a/program/1S3B/RawData/Item_Data.xlsx
+++ b/program/1S3B/RawData/Item_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\STIKA\Unity\1S3B\program\1S3B\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8659A92-25EA-4A28-B5CA-02951F0487D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5B6038-44D4-4DCC-A4FB-B1F9DB8BB65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28965" yWindow="990" windowWidth="23460" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="124">
   <si>
     <t>Water</t>
   </si>
@@ -403,6 +403,22 @@
   </si>
   <si>
     <t>DropPercent</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>손</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 상태</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Equip</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hand</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1027,10 +1043,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1089,21 +1105,21 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
-        <v>1001</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>49</v>
+        <v>1000</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="G2">
         <v>-1</v>
@@ -1117,31 +1133,31 @@
       <c r="J2">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2">
-        <v>-1</v>
+      <c r="K2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="G3">
         <v>-1</v>
@@ -1159,27 +1175,27 @@
         <v>28</v>
       </c>
       <c r="L3" t="s">
-        <v>58</v>
-      </c>
-      <c r="M3">
-        <v>-1</v>
+        <v>57</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
         <v>28</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>-1</v>
@@ -1197,27 +1213,27 @@
         <v>28</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4">
-        <v>-1</v>
+        <v>58</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
         <v>28</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="G5">
         <v>-1</v>
@@ -1235,27 +1251,27 @@
         <v>28</v>
       </c>
       <c r="L5" t="s">
-        <v>60</v>
-      </c>
-      <c r="M5">
-        <v>-1</v>
+        <v>33</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="E6" t="s">
         <v>28</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="G6">
         <v>-1</v>
@@ -1273,56 +1289,56 @@
         <v>28</v>
       </c>
       <c r="L6" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>1005</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <v>-1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" t="s">
         <v>59</v>
       </c>
-      <c r="M6">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="1">
-        <v>2001</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7">
-        <v>-1</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>100</v>
-      </c>
-      <c r="K7" t="s">
-        <v>70</v>
-      </c>
-      <c r="L7" t="s">
-        <v>68</v>
-      </c>
-      <c r="M7">
-        <v>-1</v>
+      <c r="M7" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
         <v>35</v>
@@ -1334,7 +1350,7 @@
         <v>-1</v>
       </c>
       <c r="G8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1349,7 +1365,7 @@
         <v>70</v>
       </c>
       <c r="L8" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="M8">
         <v>-1</v>
@@ -1357,10 +1373,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
         <v>35</v>
@@ -1372,7 +1388,7 @@
         <v>-1</v>
       </c>
       <c r="G9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1387,7 +1403,7 @@
         <v>70</v>
       </c>
       <c r="L9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M9">
         <v>-1</v>
@@ -1395,10 +1411,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
         <v>35</v>
@@ -1410,7 +1426,7 @@
         <v>-1</v>
       </c>
       <c r="G10" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1425,7 +1441,7 @@
         <v>70</v>
       </c>
       <c r="L10" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="M10">
         <v>-1</v>
@@ -1433,10 +1449,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
         <v>35</v>
@@ -1448,7 +1464,7 @@
         <v>-1</v>
       </c>
       <c r="G11" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1463,7 +1479,7 @@
         <v>70</v>
       </c>
       <c r="L11" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="M11">
         <v>-1</v>
@@ -1471,10 +1487,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
         <v>35</v>
@@ -1486,7 +1502,7 @@
         <v>-1</v>
       </c>
       <c r="G12" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1501,7 +1517,7 @@
         <v>70</v>
       </c>
       <c r="L12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M12">
         <v>-1</v>
@@ -1509,10 +1525,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
         <v>35</v>
@@ -1524,7 +1540,7 @@
         <v>-1</v>
       </c>
       <c r="G13" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1539,18 +1555,18 @@
         <v>70</v>
       </c>
       <c r="L13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M13">
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
-        <v>3001</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>2007</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
       </c>
       <c r="D14" t="s">
         <v>35</v>
@@ -1562,7 +1578,7 @@
         <v>-1</v>
       </c>
       <c r="G14" s="1">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1577,18 +1593,18 @@
         <v>70</v>
       </c>
       <c r="L14" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="M14">
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
-        <v>3002</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
+        <v>3001</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D15" t="s">
         <v>35</v>
@@ -1600,7 +1616,7 @@
         <v>-1</v>
       </c>
       <c r="G15" s="1">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1615,7 +1631,7 @@
         <v>70</v>
       </c>
       <c r="L15" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="M15">
         <v>-1</v>
@@ -1623,10 +1639,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
-        <v>3003</v>
+        <v>3002</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
         <v>35</v>
@@ -1638,7 +1654,7 @@
         <v>-1</v>
       </c>
       <c r="G16" s="1">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1653,7 +1669,7 @@
         <v>70</v>
       </c>
       <c r="L16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="M16">
         <v>-1</v>
@@ -1661,10 +1677,10 @@
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
-        <v>3004</v>
+        <v>3003</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
         <v>35</v>
@@ -1676,7 +1692,7 @@
         <v>-1</v>
       </c>
       <c r="G17" s="1">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1691,7 +1707,7 @@
         <v>70</v>
       </c>
       <c r="L17" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="M17">
         <v>-1</v>
@@ -1699,22 +1715,22 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
-        <v>4001</v>
+        <v>3004</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F18">
         <v>-1</v>
       </c>
-      <c r="G18">
-        <v>-1</v>
+      <c r="G18" s="1">
+        <v>104</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1726,10 +1742,10 @@
         <v>100</v>
       </c>
       <c r="K18" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="L18" t="s">
-        <v>5</v>
+        <v>79</v>
       </c>
       <c r="M18">
         <v>-1</v>
@@ -1737,13 +1753,13 @@
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
-        <v>4011</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>113</v>
+        <v>4001</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
       </c>
       <c r="E19" t="s">
         <v>26</v>
@@ -1767,21 +1783,21 @@
         <v>26</v>
       </c>
       <c r="L19" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M19">
-        <v>50</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
-        <v>4012</v>
+        <v>4011</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E20" t="s">
         <v>26</v>
@@ -1804,22 +1820,22 @@
       <c r="K20" t="s">
         <v>26</v>
       </c>
-      <c r="L20" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="M20" s="3">
-        <v>20</v>
+      <c r="L20" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20">
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
-        <v>4013</v>
+        <v>4012</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E21" t="s">
         <v>26</v>
@@ -1843,21 +1859,21 @@
         <v>26</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="M21" s="3">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
-        <v>4014</v>
+        <v>4013</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E22" t="s">
         <v>26</v>
@@ -1881,21 +1897,21 @@
         <v>26</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M22" s="3">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
-        <v>4015</v>
+        <v>4014</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E23" t="s">
         <v>26</v>
@@ -1919,24 +1935,24 @@
         <v>26</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M23" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
-        <v>5001</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>13</v>
+        <v>4015</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="E24" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="F24">
         <v>-1</v>
@@ -1953,25 +1969,25 @@
       <c r="J24">
         <v>100</v>
       </c>
-      <c r="K24" s="3" t="s">
-        <v>88</v>
+      <c r="K24" t="s">
+        <v>26</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="M24">
-        <v>-1</v>
+        <v>110</v>
+      </c>
+      <c r="M24" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
-        <v>5002</v>
+        <v>5001</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="E25" t="s">
         <v>2</v>
@@ -1995,7 +2011,7 @@
         <v>88</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M25">
         <v>-1</v>
@@ -2003,10 +2019,10 @@
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D26" t="s">
         <v>41</v>
@@ -2033,7 +2049,7 @@
         <v>88</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M26">
         <v>-1</v>
@@ -2041,7 +2057,7 @@
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
-        <v>5004</v>
+        <v>5003</v>
       </c>
       <c r="C27" t="s">
         <v>44</v>
@@ -2071,7 +2087,7 @@
         <v>88</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M27">
         <v>-1</v>
@@ -2079,7 +2095,7 @@
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
-        <v>5005</v>
+        <v>5004</v>
       </c>
       <c r="C28" t="s">
         <v>44</v>
@@ -2109,7 +2125,7 @@
         <v>88</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M28">
         <v>-1</v>
@@ -2117,7 +2133,7 @@
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" s="1">
-        <v>5006</v>
+        <v>5005</v>
       </c>
       <c r="C29" t="s">
         <v>44</v>
@@ -2147,7 +2163,7 @@
         <v>88</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M29">
         <v>-1</v>
@@ -2155,10 +2171,10 @@
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B30" s="1">
-        <v>5007</v>
+        <v>5006</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D30" t="s">
         <v>41</v>
@@ -2185,7 +2201,7 @@
         <v>88</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M30">
         <v>-1</v>
@@ -2193,13 +2209,13 @@
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B31" s="1">
-        <v>5101</v>
+        <v>5007</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="E31" t="s">
         <v>2</v>
@@ -2223,7 +2239,7 @@
         <v>88</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M31">
         <v>-1</v>
@@ -2231,13 +2247,13 @@
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B32" s="1">
-        <v>5102</v>
+        <v>5101</v>
       </c>
       <c r="C32" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="E32" t="s">
         <v>2</v>
@@ -2261,7 +2277,7 @@
         <v>88</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M32">
         <v>-1</v>
@@ -2269,10 +2285,10 @@
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B33" s="1">
-        <v>5103</v>
+        <v>5102</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D33" t="s">
         <v>39</v>
@@ -2299,7 +2315,7 @@
         <v>88</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="M33">
         <v>-1</v>
@@ -2307,7 +2323,7 @@
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B34" s="1">
-        <v>5104</v>
+        <v>5103</v>
       </c>
       <c r="C34" t="s">
         <v>44</v>
@@ -2337,7 +2353,7 @@
         <v>88</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M34">
         <v>-1</v>
@@ -2345,7 +2361,7 @@
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B35" s="1">
-        <v>5105</v>
+        <v>5104</v>
       </c>
       <c r="C35" t="s">
         <v>44</v>
@@ -2375,7 +2391,7 @@
         <v>88</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M35">
         <v>-1</v>
@@ -2383,7 +2399,7 @@
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B36" s="1">
-        <v>5106</v>
+        <v>5105</v>
       </c>
       <c r="C36" t="s">
         <v>44</v>
@@ -2413,7 +2429,7 @@
         <v>88</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M36">
         <v>-1</v>
@@ -2421,13 +2437,13 @@
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B37" s="1">
-        <v>5201</v>
+        <v>5106</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="E37" t="s">
         <v>2</v>
@@ -2451,7 +2467,7 @@
         <v>88</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="M37">
         <v>-1</v>
@@ -2459,13 +2475,13 @@
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B38" s="1">
-        <v>5202</v>
+        <v>5201</v>
       </c>
       <c r="C38" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="E38" t="s">
         <v>2</v>
@@ -2489,7 +2505,7 @@
         <v>88</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M38">
         <v>-1</v>
@@ -2497,7 +2513,7 @@
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B39" s="1">
-        <v>5203</v>
+        <v>5202</v>
       </c>
       <c r="C39" t="s">
         <v>44</v>
@@ -2527,7 +2543,7 @@
         <v>88</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="M39">
         <v>-1</v>
@@ -2535,7 +2551,7 @@
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B40" s="1">
-        <v>5204</v>
+        <v>5203</v>
       </c>
       <c r="C40" t="s">
         <v>44</v>
@@ -2565,7 +2581,7 @@
         <v>88</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M40">
         <v>-1</v>
@@ -2573,7 +2589,7 @@
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B41" s="1">
-        <v>5205</v>
+        <v>5204</v>
       </c>
       <c r="C41" t="s">
         <v>44</v>
@@ -2603,7 +2619,7 @@
         <v>88</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M41">
         <v>-1</v>
@@ -2611,13 +2627,13 @@
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B42" s="1">
-        <v>5206</v>
+        <v>5205</v>
       </c>
       <c r="C42" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D42" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="E42" t="s">
         <v>2</v>
@@ -2641,7 +2657,7 @@
         <v>88</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M42">
         <v>-1</v>
@@ -2649,13 +2665,13 @@
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B43" s="1">
-        <v>5301</v>
+        <v>5206</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E43" t="s">
         <v>2</v>
@@ -2679,7 +2695,7 @@
         <v>88</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="M43">
         <v>-1</v>
@@ -2687,13 +2703,13 @@
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B44" s="1">
-        <v>5302</v>
+        <v>5301</v>
       </c>
       <c r="C44" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="E44" t="s">
         <v>2</v>
@@ -2717,7 +2733,7 @@
         <v>88</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M44">
         <v>-1</v>
@@ -2725,7 +2741,7 @@
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B45" s="1">
-        <v>5303</v>
+        <v>5302</v>
       </c>
       <c r="C45" t="s">
         <v>44</v>
@@ -2755,7 +2771,7 @@
         <v>88</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="M45">
         <v>-1</v>
@@ -2763,7 +2779,7 @@
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B46" s="1">
-        <v>5304</v>
+        <v>5303</v>
       </c>
       <c r="C46" t="s">
         <v>44</v>
@@ -2793,9 +2809,47 @@
         <v>88</v>
       </c>
       <c r="L46" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="M46">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B47" s="1">
+        <v>5304</v>
+      </c>
+      <c r="C47" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <v>-1</v>
+      </c>
+      <c r="G47">
+        <v>-1</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>100</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="L47" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="M46">
+      <c r="M47">
         <v>-1</v>
       </c>
     </row>

</xml_diff>